<commit_message>
add performance analyze excel
</commit_message>
<xml_diff>
--- a/doc/perf/SM3性能分析.xlsx
+++ b/doc/perf/SM3性能分析.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>SM3_core 性能分析</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,6 +83,10 @@
   </si>
   <si>
     <t>FPGA：V7 (xc7vx330t) / Vivad0 18.3/默认策略</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手动CSA加法器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -413,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -549,38 +553,116 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>-0.2</v>
+        <v>-3.6850000000000001</v>
       </c>
       <c r="E6">
         <f>C6-D6</f>
-        <v>4.2</v>
+        <v>6.6850000000000005</v>
       </c>
       <c r="F6">
         <f>1/E6*1000</f>
+        <v>149.58863126402392</v>
+      </c>
+      <c r="G6">
+        <f>512/(33*E6)</f>
+        <v>2.3208902790054622</v>
+      </c>
+      <c r="H6">
+        <f>E6*33</f>
+        <v>220.60500000000002</v>
+      </c>
+      <c r="I6">
+        <v>1795</v>
+      </c>
+      <c r="J6">
+        <v>552</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>-0.2</v>
+      </c>
+      <c r="E7">
+        <f>C7-D7</f>
+        <v>4.2</v>
+      </c>
+      <c r="F7">
+        <f>1/E7*1000</f>
         <v>238.09523809523807</v>
       </c>
-      <c r="G6">
-        <f>512/(65*E6)</f>
+      <c r="G7">
+        <f>512/(65*E7)</f>
         <v>1.8754578754578755</v>
       </c>
-      <c r="H6">
-        <f>E6*65</f>
+      <c r="H7">
+        <f>E7*65</f>
         <v>273</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>1224</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <v>418</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>-0.61699999999999999</v>
+      </c>
+      <c r="E8">
+        <f>C8-D8</f>
+        <v>3.617</v>
+      </c>
+      <c r="F8">
+        <f>1/E8*1000</f>
+        <v>276.47221454243845</v>
+      </c>
+      <c r="G8">
+        <f>512/(65*E8)</f>
+        <v>2.1777503668573619</v>
+      </c>
+      <c r="H8">
+        <f>E8*65</f>
+        <v>235.10499999999999</v>
+      </c>
+      <c r="I8">
+        <v>1369</v>
+      </c>
+      <c r="J8">
+        <v>457</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>